<commit_message>
finish proposal after talking to Dr. Pauchard
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6ad8ef6fe9c5877e/Documents/School/MEng/Semester 3/ENSF 611/Assignments/ml-project-GraydonHall42/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{896BC6C6-BC4D-46F4-91B3-0E74F8399496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{896BC6C6-BC4D-46F4-91B3-0E74F8399496}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4F2CED0-3FDF-40CA-99D8-298AC1C9D1FC}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3A0D84DB-2915-42E1-934E-3C45891C8EF7}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="21">
   <si>
     <t>GradientBoostingClassifier</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>Section 6 results</t>
+  </si>
+  <si>
+    <t>Test Score</t>
   </si>
 </sst>
 </file>
@@ -101,7 +104,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -282,12 +285,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -303,6 +300,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,51 +359,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +677,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -699,169 +702,169 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="3" t="s">
+      <c r="A2" s="3"/>
+      <c r="B2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10" t="s">
+      <c r="E2" s="24"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="11"/>
-      <c r="K2" s="12"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="13" t="s">
+      <c r="H3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="13" t="s">
+      <c r="I3" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="K3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="12">
         <v>0.96299999999999997</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="12">
         <v>0.85399999999999998</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="12">
         <v>0.93500000000000005</v>
       </c>
-      <c r="E4" s="18">
+      <c r="E4" s="13">
         <v>0.82699999999999996</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="9">
         <v>0.90500000000000003</v>
       </c>
-      <c r="J4" s="14">
+      <c r="J4" s="9">
         <v>0.84399999999999997</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="9" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="12">
         <v>0.878</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="12">
         <v>0.85799999999999998</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="12">
         <v>0.83499999999999996</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E5" s="13">
         <v>0.81499999999999995</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="9">
         <v>0.95699999999999996</v>
       </c>
-      <c r="J5" s="14">
+      <c r="J5" s="9">
         <v>0.83399999999999996</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="12">
         <v>0.85799999999999998</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="12">
         <v>0.85699999999999998</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="12">
         <v>0.80700000000000005</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="13">
         <v>0.81299999999999994</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="I6" s="15">
+      <c r="I6" s="10">
         <v>0.85899999999999999</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="10">
         <v>0.82699999999999996</v>
       </c>
-      <c r="K6" s="8" t="s">
+      <c r="K6" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="12">
         <v>0.999</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="12">
         <v>0.83599999999999997</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="12">
         <v>0.996</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="13">
         <v>0.80800000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="14">
         <v>0.81799999999999995</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="14">
         <v>0.81599999999999995</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="14">
         <v>0.77800000000000002</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="15">
         <v>0.77200000000000002</v>
       </c>
     </row>
@@ -874,98 +877,98 @@
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="3" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3" t="s">
+      <c r="C12" s="24"/>
+      <c r="D12" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="24"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6" t="s">
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>8</v>
+      <c r="E13" s="4" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="22">
+      <c r="B14" s="17">
         <v>0.89</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="17">
         <v>0.78</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="17">
         <v>0.89</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="18">
         <v>0.84</v>
       </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="19">
         <v>0.98</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="19">
         <v>0.8</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="19">
         <v>0.96</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="20">
         <v>0.85</v>
       </c>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="19">
         <v>0.96</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16" s="19">
         <v>0.78</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="19">
         <v>0.95</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="20">
         <v>0.85</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A17" s="8" t="s">
+      <c r="A17" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="26">
+      <c r="B17" s="21">
         <v>0.96</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="21">
         <v>0.78</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="21">
         <v>0.95</v>
       </c>
-      <c r="E17" s="27">
+      <c r="E17" s="22">
         <v>0.85</v>
       </c>
     </row>

</xml_diff>